<commit_message>
add new extracted rob and merge with studylist
</commit_message>
<xml_diff>
--- a/02_data/cleandata/df_rob_clean.xlsx
+++ b/02_data/cleandata/df_rob_clean.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S130"/>
+  <dimension ref="A1:S140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -11232,6 +11232,876 @@
         </is>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Barrowclough(2015)</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>Barrowclough</t>
+        </is>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>Barrowclough</t>
+        </is>
+      </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>barrowclough_2015</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Barrowclough(2013)</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P132" t="inlineStr">
+        <is>
+          <t>Barrowclough</t>
+        </is>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>Barrowclough</t>
+        </is>
+      </c>
+      <c r="R132" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>barrowclough_2013</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Fond(2019)</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P133" t="inlineStr">
+        <is>
+          <t>Fond</t>
+        </is>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>Fond</t>
+        </is>
+      </c>
+      <c r="R133" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>fond_2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Foti(2010)</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P134" t="inlineStr">
+        <is>
+          <t>Foti</t>
+        </is>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>Foti</t>
+        </is>
+      </c>
+      <c r="R134" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>foti_2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Baeza(2009)</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P135" t="inlineStr">
+        <is>
+          <t>Baeza</t>
+        </is>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>Baeza</t>
+        </is>
+      </c>
+      <c r="R135" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>baeza_2009</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Buchy(2015)</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P136" t="inlineStr">
+        <is>
+          <t>Buchy</t>
+        </is>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>Buchy</t>
+        </is>
+      </c>
+      <c r="R136" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>buchy_2015</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Zammit(2011)</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P137" t="inlineStr">
+        <is>
+          <t>Zammit</t>
+        </is>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>Zammit</t>
+        </is>
+      </c>
+      <c r="R137" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>zammit_2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Arseneault(2002)</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P138" t="inlineStr">
+        <is>
+          <t>Arseneault</t>
+        </is>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>Arseneault</t>
+        </is>
+      </c>
+      <c r="R138" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>arseneault_2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Bechtold(2016)</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P139" t="inlineStr">
+        <is>
+          <t>Bechtold</t>
+        </is>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>Bechtold</t>
+        </is>
+      </c>
+      <c r="R139" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>bechtold_2016</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Rob_HPP_J</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Dragt(2011)</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>longitudinal prospective</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>Johanna</t>
+        </is>
+      </c>
+      <c r="P140" t="inlineStr">
+        <is>
+          <t>Dragt</t>
+        </is>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>Dragt</t>
+        </is>
+      </c>
+      <c r="R140" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>dragt_2011</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>